<commit_message>
backup BI - list sharepoint
</commit_message>
<xml_diff>
--- a/Base De dados almocharifado.xlsx
+++ b/Base De dados almocharifado.xlsx
@@ -5,16 +5,17 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micael.amaral\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micael.amaral\Documents\projeto_BI-ALMOXARIFADO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F38506FE-8935-4B7B-B908-3BD2EA6D9F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB6E514-7377-4112-B4E5-042617782701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela Uniforme Masculino" sheetId="1" r:id="rId1"/>
     <sheet name="Tabela Uniformes feminina" sheetId="10" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t xml:space="preserve">Camisa Manga Longa </t>
   </si>
@@ -135,9 +136,6 @@
     <t>Uniforme Fiscalização 2ª  Pele</t>
   </si>
   <si>
-    <t>TAMAHOS</t>
-  </si>
-  <si>
     <t>TAMANHOS</t>
   </si>
   <si>
@@ -147,9 +145,6 @@
     <t xml:space="preserve"> Uniforme Fiscalização Calça</t>
   </si>
   <si>
-    <t xml:space="preserve">Camissa Fiscalição Manga Curta </t>
-  </si>
-  <si>
     <t>TAMANHO</t>
   </si>
   <si>
@@ -157,6 +152,24 @@
   </si>
   <si>
     <t>Camisa  Fiscalização Agasalho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camisa Fiscalição Manga Curta </t>
+  </si>
+  <si>
+    <t>PROCESSO SEI</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>QUANTIDADE</t>
   </si>
 </sst>
 </file>
@@ -167,7 +180,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,8 +230,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +274,12 @@
       <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -399,7 +434,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -443,66 +478,65 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="5" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -511,10 +545,10 @@
     <cellStyle name="Ênfase3" xfId="2" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="30">
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -524,103 +558,18 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FFFFFFFF"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -741,6 +690,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -748,12 +703,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -882,42 +831,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -937,6 +850,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0" tint="-0.14999847407452621"/>
@@ -944,6 +858,90 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1202,6 +1200,67 @@
         </right>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1216,27 +1275,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6799E189-80AD-4CD7-B04E-719B36AB7C3D}" name="TabelaMasculinoNUMERO" displayName="TabelaMasculinoNUMERO" ref="A1:G16" totalsRowShown="0" headerRowDxfId="20" dataDxfId="21" tableBorderDxfId="28" headerRowCellStyle="Ênfase3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6799E189-80AD-4CD7-B04E-719B36AB7C3D}" name="TabelaMasculinoNUMERO" displayName="TabelaMasculinoNUMERO" ref="A1:G16" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" headerRowCellStyle="Ênfase3">
   <autoFilter ref="A1:G16" xr:uid="{6799E189-80AD-4CD7-B04E-719B36AB7C3D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1C8E3BA8-2099-4CBF-A5C1-37755692A9EE}" name="TAMAHOS"/>
-    <tableColumn id="2" xr3:uid="{F7132A4D-8B48-4405-BB76-35946031D193}" name="Camissa Fiscalição Manga Curta " dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{60B7B1FC-4D53-453C-96D0-9E3BCFB03AFE}" name=" Camisa Fiscalização Agasalho " dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{4B44547D-259E-482C-BE7C-66F410E00BC0}" name=" Uniforme Fiscalização Calça" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{EB51DAFB-1FA8-4731-9F89-8CB6989390FE}" name="Camisa Manga Longa " dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{BE16310C-19F4-445E-B7C4-F44856E4A5B3}" name="Camisa Fiscalização Gandola" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{7AA6EDD9-96AE-4F7C-A9D6-5F5323115F4B}" name="Camisa Fiscalização Gola Polo" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{1C8E3BA8-2099-4CBF-A5C1-37755692A9EE}" name="TAMANHOS"/>
+    <tableColumn id="2" xr3:uid="{F7132A4D-8B48-4405-BB76-35946031D193}" name="Camisa Fiscalição Manga Curta " dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{60B7B1FC-4D53-453C-96D0-9E3BCFB03AFE}" name=" Camisa Fiscalização Agasalho " dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{4B44547D-259E-482C-BE7C-66F410E00BC0}" name=" Uniforme Fiscalização Calça" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{EB51DAFB-1FA8-4731-9F89-8CB6989390FE}" name="Camisa Manga Longa " dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{BE16310C-19F4-445E-B7C4-F44856E4A5B3}" name="Camisa Fiscalização Gandola" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{7AA6EDD9-96AE-4F7C-A9D6-5F5323115F4B}" name="Camisa Fiscalização Gola Polo" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B6FFA5FD-19B4-40F9-8BD7-C1C1DE12741A}" name="TabelaMasculinoLETRA" displayName="TabelaMasculinoLETRA" ref="A18:B29" totalsRowShown="0" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B6FFA5FD-19B4-40F9-8BD7-C1C1DE12741A}" name="TabelaMasculinoLETRA" displayName="TabelaMasculinoLETRA" ref="A18:B29" totalsRowShown="0" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="A18:B29" xr:uid="{B6FFA5FD-19B4-40F9-8BD7-C1C1DE12741A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FFD3FF00-DD23-47D6-97C2-61128FA826B0}" name="TAMANHOS" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{42FB880F-0AF4-4A89-8646-18C2B683BCEC}" name="Uniforme Fiscalização 2ª  Pele" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FFD3FF00-DD23-47D6-97C2-61128FA826B0}" name="TAMANHOS" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{42FB880F-0AF4-4A89-8646-18C2B683BCEC}" name="Uniforme Fiscalização 2ª  Pele" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1246,24 +1305,39 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C9D4BEE-66AA-48F0-B386-E1EC56C02F26}" name="TabelaFemininoNUMERO" displayName="TabelaFemininoNUMERO" ref="A1:G14" totalsRowShown="0">
   <autoFilter ref="A1:G14" xr:uid="{8C9D4BEE-66AA-48F0-B386-E1EC56C02F26}"/>
   <tableColumns count="7">
-    <tableColumn id="3" xr3:uid="{1865ADE4-2705-44EC-A1AA-23C38CFBA5BE}" name="TAMANHO" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{C9477343-46E3-40F8-9B67-420B68938A83}" name="Fiscalição Manga Curta" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{B886A1C8-7F54-4B1A-A5F9-BCCEF137521A}" name="Camisa  Fiscalização Agasalho" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{D16174EA-E069-4E35-A36D-24F3DD3B70B1}" name="Uniforme Fiscalização Calça" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{CBEC5BA1-E0CC-444C-8A53-1564080B77B2}" name="Camisa Manga Longa " dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{211FC2F5-8670-412C-BCDF-1163F01AB8AE}" name="Camisa Fiscalização Gandola" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{B07406A3-052F-4C64-8F4B-EE5DB6EB3C4C}" name="Camisa Fiscalização Gola Polo" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{1865ADE4-2705-44EC-A1AA-23C38CFBA5BE}" name="TAMANHO" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{C9477343-46E3-40F8-9B67-420B68938A83}" name="Fiscalição Manga Curta" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{B886A1C8-7F54-4B1A-A5F9-BCCEF137521A}" name="Camisa  Fiscalização Agasalho" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{D16174EA-E069-4E35-A36D-24F3DD3B70B1}" name="Uniforme Fiscalização Calça" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{CBEC5BA1-E0CC-444C-8A53-1564080B77B2}" name="Camisa Manga Longa " dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{211FC2F5-8670-412C-BCDF-1163F01AB8AE}" name="Camisa Fiscalização Gandola" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{B07406A3-052F-4C64-8F4B-EE5DB6EB3C4C}" name="Camisa Fiscalização Gola Polo" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{042F0858-6A5D-4AC5-BFF6-CF0F3D14445F}" name="TabelaFemininoLETRA" displayName="TabelaFemininoLETRA" ref="A16:B27" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{042F0858-6A5D-4AC5-BFF6-CF0F3D14445F}" name="TabelaFemininoLETRA" displayName="TabelaFemininoLETRA" ref="A16:B27" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A16:B27" xr:uid="{042F0858-6A5D-4AC5-BFF6-CF0F3D14445F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C1602BAA-A078-4696-A69E-98F15358263F}" name="TAMANHO" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{11EEBF1E-DB26-4656-BD5A-D96439487231}" name="Uniforme Fiscalização 2ª  Pele" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{C1602BAA-A078-4696-A69E-98F15358263F}" name="TAMANHO" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{11EEBF1E-DB26-4656-BD5A-D96439487231}" name="Uniforme Fiscalização 2ª  Pele" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F03FC937-3BC8-489F-BAFD-8BBF4FED3632}" name="Tabela7" displayName="Tabela7" ref="A1:F2" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F2" xr:uid="{F03FC937-3BC8-489F-BAFD-8BBF4FED3632}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{DA5CCEA5-F6DC-4832-86A1-04D61EE74479}" name="PROCESSO SEI"/>
+    <tableColumn id="2" xr3:uid="{A2530B8C-C557-47B6-9AEC-98F9C07FBBC1}" name="NOME"/>
+    <tableColumn id="3" xr3:uid="{D7764219-75E3-4913-8393-DF560AC31182}" name="DATA"/>
+    <tableColumn id="4" xr3:uid="{0E970F9A-AF2B-4E34-A891-83933D0A331F}" name="ITEM"/>
+    <tableColumn id="5" xr3:uid="{55090423-684E-4296-8EF1-E1341F3065A6}" name="TAMANHO"/>
+    <tableColumn id="6" xr3:uid="{ADE5F247-ABE3-4D49-9803-B8D659E7BF8C}" name="QUANTIDADE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1588,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,25 +1687,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="37" t="s">
+      <c r="E1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="35" t="s">
         <v>30</v>
       </c>
       <c r="H1"/>
@@ -1648,22 +1722,22 @@
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="23">
         <v>2</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="23">
         <v>9</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="23">
         <v>7</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="23">
         <v>1</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="23">
         <v>6</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="25">
         <v>12</v>
       </c>
       <c r="H2"/>
@@ -1677,25 +1751,25 @@
       <c r="P2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="23">
-        <v>0</v>
-      </c>
-      <c r="C3" s="23">
+      <c r="B3" s="22">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22">
         <v>7</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="22">
         <v>5</v>
       </c>
-      <c r="E3" s="23">
-        <v>0</v>
-      </c>
-      <c r="F3" s="23">
+      <c r="E3" s="22">
+        <v>0</v>
+      </c>
+      <c r="F3" s="22">
         <v>5</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="27">
         <v>20</v>
       </c>
       <c r="H3"/>
@@ -1712,22 +1786,22 @@
       <c r="A4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="23">
-        <v>0</v>
-      </c>
-      <c r="C4" s="23">
+      <c r="B4" s="22">
+        <v>0</v>
+      </c>
+      <c r="C4" s="22">
         <v>39</v>
       </c>
-      <c r="D4" s="23">
-        <v>0</v>
-      </c>
-      <c r="E4" s="23">
-        <v>0</v>
-      </c>
-      <c r="F4" s="23">
+      <c r="D4" s="22">
+        <v>0</v>
+      </c>
+      <c r="E4" s="22">
+        <v>0</v>
+      </c>
+      <c r="F4" s="22">
         <v>3</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="27">
         <v>34</v>
       </c>
       <c r="H4"/>
@@ -1741,25 +1815,25 @@
       <c r="P4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="22">
         <v>1</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22">
         <v>67</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <v>26</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>135</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <v>30</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="27">
         <v>55</v>
       </c>
       <c r="H5"/>
@@ -1773,25 +1847,25 @@
       <c r="P5"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>92</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="22">
         <v>21</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="22">
         <v>52</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <v>81</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="22">
         <v>54</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="27">
         <v>30</v>
       </c>
       <c r="H6"/>
@@ -1808,22 +1882,22 @@
       <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>94</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="22">
         <v>21</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <v>15</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <v>95</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="22">
         <v>17</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="27">
         <v>104</v>
       </c>
       <c r="H7"/>
@@ -1840,22 +1914,22 @@
       <c r="A8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>83</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="22">
         <v>25</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="22">
         <v>24</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <v>79</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="22">
         <v>31</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="27">
         <v>11</v>
       </c>
       <c r="H8"/>
@@ -1872,22 +1946,22 @@
       <c r="A9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="22">
         <v>50</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="22">
         <v>1</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="22">
         <v>120</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="22">
         <v>27</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="22">
         <v>39</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="27">
         <v>36</v>
       </c>
       <c r="H9"/>
@@ -1901,25 +1975,25 @@
       <c r="P9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>31</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="22">
         <v>1</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <v>14</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <v>36</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="22">
         <v>2</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="27">
         <v>48</v>
       </c>
       <c r="H10"/>
@@ -1936,22 +2010,22 @@
       <c r="A11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="22">
         <v>14</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="22">
         <v>6</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="22">
         <v>4</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="22">
         <v>19</v>
       </c>
-      <c r="F11" s="23">
-        <v>0</v>
-      </c>
-      <c r="G11" s="29">
+      <c r="F11" s="22">
+        <v>0</v>
+      </c>
+      <c r="G11" s="27">
         <v>30</v>
       </c>
       <c r="H11"/>
@@ -1965,25 +2039,25 @@
       <c r="P11"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="22">
         <v>5</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="22">
         <v>7</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <v>7</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="22">
         <v>1</v>
       </c>
-      <c r="F12" s="23">
-        <v>0</v>
-      </c>
-      <c r="G12" s="29">
+      <c r="F12" s="22">
+        <v>0</v>
+      </c>
+      <c r="G12" s="27">
         <v>96</v>
       </c>
       <c r="H12"/>
@@ -2000,22 +2074,22 @@
       <c r="A13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="23">
-        <v>0</v>
-      </c>
-      <c r="C13" s="23">
-        <v>0</v>
-      </c>
-      <c r="D13" s="23">
+      <c r="B13" s="22">
+        <v>0</v>
+      </c>
+      <c r="C13" s="22">
+        <v>0</v>
+      </c>
+      <c r="D13" s="22">
         <v>8</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <v>2</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="22">
         <v>15</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="27">
         <v>39</v>
       </c>
       <c r="H13"/>
@@ -2032,22 +2106,22 @@
       <c r="A14" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="23">
-        <v>0</v>
-      </c>
-      <c r="C14" s="23">
-        <v>0</v>
-      </c>
-      <c r="D14" s="23">
-        <v>0</v>
-      </c>
-      <c r="E14" s="23">
-        <v>0</v>
-      </c>
-      <c r="F14" s="23">
-        <v>0</v>
-      </c>
-      <c r="G14" s="29">
+      <c r="B14" s="22">
+        <v>0</v>
+      </c>
+      <c r="C14" s="22">
+        <v>0</v>
+      </c>
+      <c r="D14" s="22">
+        <v>0</v>
+      </c>
+      <c r="E14" s="22">
+        <v>0</v>
+      </c>
+      <c r="F14" s="22">
+        <v>0</v>
+      </c>
+      <c r="G14" s="27">
         <v>39</v>
       </c>
       <c r="H14"/>
@@ -2064,22 +2138,22 @@
       <c r="A15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="24">
-        <v>0</v>
-      </c>
-      <c r="C15" s="24">
-        <v>0</v>
-      </c>
-      <c r="D15" s="24">
-        <v>0</v>
-      </c>
-      <c r="E15" s="24">
-        <v>0</v>
-      </c>
-      <c r="F15" s="24">
-        <v>0</v>
-      </c>
-      <c r="G15" s="28">
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="26">
         <v>77</v>
       </c>
       <c r="H15"/>
@@ -2093,25 +2167,25 @@
       <c r="P15"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="23">
-        <v>0</v>
-      </c>
-      <c r="C16" s="23">
-        <v>0</v>
-      </c>
-      <c r="D16" s="23">
-        <v>0</v>
-      </c>
-      <c r="E16" s="23">
-        <v>0</v>
-      </c>
-      <c r="F16" s="26">
-        <v>0</v>
-      </c>
-      <c r="G16" s="30">
+      <c r="B16" s="22">
+        <v>0</v>
+      </c>
+      <c r="C16" s="22">
+        <v>0</v>
+      </c>
+      <c r="D16" s="22">
+        <v>0</v>
+      </c>
+      <c r="E16" s="22">
+        <v>0</v>
+      </c>
+      <c r="F16" s="24">
+        <v>0</v>
+      </c>
+      <c r="G16" s="28">
         <v>54</v>
       </c>
       <c r="H16"/>
@@ -2128,98 +2202,98 @@
       <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="27">
         <v>33</v>
       </c>
-      <c r="B18" s="40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="29">
-        <v>33</v>
-      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="26">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="27">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="26">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="27">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="26">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="27">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="28">
+      <c r="B26" s="26">
         <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B27" s="27">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="28">
+      <c r="B28" s="26">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="36">
+      <c r="B29" s="34">
         <v>13</v>
       </c>
     </row>
@@ -2231,18 +2305,18 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="E2 C2:C12 G2:G16 E5:E13 B2 B19:B29 B5:B12 A2:A12">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+  <conditionalFormatting sqref="B2:B12">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B4">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+  <conditionalFormatting sqref="E2 A2:A12 C2:C12 G2:G16 E5:E13 B19:B29">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F6">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2282,13 +2356,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>39</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>29</v>
@@ -2521,7 +2595,7 @@
       <c r="N8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="4">
@@ -2707,10 +2781,10 @@
       <c r="E15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="34" t="s">
+      <c r="A16" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="32" t="s">
         <v>31</v>
       </c>
       <c r="C16"/>
@@ -2718,10 +2792,10 @@
       <c r="E16"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="27">
         <v>22</v>
       </c>
       <c r="C17"/>
@@ -2729,10 +2803,10 @@
       <c r="E17"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="26">
         <v>20</v>
       </c>
       <c r="C18"/>
@@ -2740,89 +2814,86 @@
       <c r="E18"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="27">
         <v>6</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="26">
         <v>1</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="27">
         <v>17</v>
       </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="26">
         <v>41</v>
       </c>
       <c r="D22" s="5"/>
       <c r="O22" s="3"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="27">
         <v>41</v>
       </c>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="26">
         <v>17</v>
       </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="27">
         <v>2</v>
       </c>
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="28">
+      <c r="B26" s="26">
         <v>3</v>
       </c>
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="36">
+      <c r="B27" s="34">
         <v>1</v>
       </c>
       <c r="D27" s="5"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="38"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
@@ -2856,27 +2927,51 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA414120-9A26-4606-A6A2-5A96B06CA6AA}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="818d3acb-fc29-4417-9cca-35c1337d67c6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9b1490c3-40b2-4840-b30b-837525c64aa3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000C86D41370099C438C053DFBEA28BC81" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="818ec94b270468afdd50d37653a3d272">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b1490c3-40b2-4840-b30b-837525c64aa3" xmlns:ns3="818d3acb-fc29-4417-9cca-35c1337d67c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f05552b3873356689eea1e3c2e917b82" ns2:_="" ns3:_="">
     <xsd:import namespace="9b1490c3-40b2-4840-b30b-837525c64aa3"/>
@@ -3077,10 +3172,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="818d3acb-fc29-4417-9cca-35c1337d67c6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9b1490c3-40b2-4840-b30b-837525c64aa3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA6A710C-3A0C-4088-8BD9-18F4BD1608F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48942057-5A33-465A-8624-BB46163CAD5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9b1490c3-40b2-4840-b30b-837525c64aa3"/>
+    <ds:schemaRef ds:uri="818d3acb-fc29-4417-9cca-35c1337d67c6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3097,20 +3223,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48942057-5A33-465A-8624-BB46163CAD5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA6A710C-3A0C-4088-8BD9-18F4BD1608F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9b1490c3-40b2-4840-b30b-837525c64aa3"/>
-    <ds:schemaRef ds:uri="818d3acb-fc29-4417-9cca-35c1337d67c6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>